<commit_message>
calc fix first tries
</commit_message>
<xml_diff>
--- a/src/main/resources/import_test_data/supplier1_two_invoices.xlsx
+++ b/src/main/resources/import_test_data/supplier1_two_invoices.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,15 +16,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>supplier1</t>
   </si>
   <si>
-    <t>09.08.2016</t>
+    <t>1fa</t>
   </si>
   <si>
-    <t>28.08.2016</t>
+    <t>1ddd</t>
+  </si>
+  <si>
+    <t>30.08.2016</t>
+  </si>
+  <si>
+    <t>30.09.2016</t>
   </si>
 </sst>
 </file>
@@ -60,11 +66,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -77,9 +88,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -117,7 +128,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -189,7 +200,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -363,38 +374,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>100</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
+      <c r="C1" s="2">
+        <v>50000</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C2" s="2">
+        <v>50000</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added checked invoices persists
</commit_message>
<xml_diff>
--- a/src/main/resources/import_test_data/supplier1_two_invoices.xlsx
+++ b/src/main/resources/import_test_data/supplier1_two_invoices.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -27,10 +27,10 @@
     <t>1ddd</t>
   </si>
   <si>
-    <t>30.08.2016</t>
+    <t>30.09.2016</t>
   </si>
   <si>
-    <t>30.09.2016</t>
+    <t>30.10.2016</t>
   </si>
 </sst>
 </file>
@@ -75,7 +75,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -88,9 +88,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -128,7 +128,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -200,7 +200,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -377,7 +377,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,7 +400,7 @@
         <v>50000</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3"/>
     </row>
@@ -415,7 +415,7 @@
         <v>50000</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="3"/>
     </row>

</xml_diff>